<commit_message>
Change order of row processing in process_excel_file
- Increase request timeouts from 15 to 20 seconds.
- Change row processing in process_excel_file to process rows in order.
- Update log message for skipped rows to mention "older rows".
</commit_message>
<xml_diff>
--- a/tests/api/data/file2.xlsx
+++ b/tests/api/data/file2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/basicthinker/Projects/devchat-webapp/tests/api/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D072DAE0-E999-754B-91D5-1E344C44A2AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84EB1F11-6381-0945-8B74-9F00E95E1AA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>Respondent Name</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>test3@merico.dev</t>
+  </si>
+  <si>
+    <t>2023-05-27 18:46:39 [UTC+08:00]</t>
   </si>
 </sst>
 </file>
@@ -471,7 +474,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -549,22 +552,25 @@
         <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>21</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -587,35 +593,32 @@
         <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H3" r:id="rId1" xr:uid="{07962994-28EF-EF42-AE81-BFB5A7C45FC9}"/>
-    <hyperlink ref="I3" r:id="rId2" xr:uid="{7C7A525D-CACC-E641-99E5-B589B5C9C310}"/>
-    <hyperlink ref="J3" r:id="rId3" xr:uid="{1A82D880-560A-B948-A784-E4522C012BFB}"/>
-    <hyperlink ref="K3" r:id="rId4" xr:uid="{6C760061-E479-6042-9BB0-D6D1ABD2C906}"/>
-    <hyperlink ref="L3" r:id="rId5" xr:uid="{BBB846C4-D4DA-B444-B083-D92411249DD7}"/>
-    <hyperlink ref="H2" r:id="rId6" xr:uid="{0333611F-D5D4-5A42-91C2-B736A8CD8336}"/>
-    <hyperlink ref="I2" r:id="rId7" xr:uid="{153F53A3-928B-784E-816E-3A75697C7B90}"/>
-    <hyperlink ref="J2" r:id="rId8" xr:uid="{A8DD6B75-9E08-CC43-B52F-404C105D1829}"/>
-    <hyperlink ref="K2" r:id="rId9" xr:uid="{651BFB58-E580-9244-BF97-CDE841D51187}"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{07962994-28EF-EF42-AE81-BFB5A7C45FC9}"/>
+    <hyperlink ref="I2" r:id="rId2" xr:uid="{7C7A525D-CACC-E641-99E5-B589B5C9C310}"/>
+    <hyperlink ref="J2" r:id="rId3" xr:uid="{1A82D880-560A-B948-A784-E4522C012BFB}"/>
+    <hyperlink ref="K2" r:id="rId4" xr:uid="{6C760061-E479-6042-9BB0-D6D1ABD2C906}"/>
+    <hyperlink ref="L2" r:id="rId5" xr:uid="{BBB846C4-D4DA-B444-B083-D92411249DD7}"/>
+    <hyperlink ref="H3" r:id="rId6" xr:uid="{0333611F-D5D4-5A42-91C2-B736A8CD8336}"/>
+    <hyperlink ref="I3" r:id="rId7" xr:uid="{153F53A3-928B-784E-816E-3A75697C7B90}"/>
+    <hyperlink ref="J3" r:id="rId8" xr:uid="{A8DD6B75-9E08-CC43-B52F-404C105D1829}"/>
+    <hyperlink ref="K3" r:id="rId9" xr:uid="{651BFB58-E580-9244-BF97-CDE841D51187}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>